<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@6a2f1fa744ccd0cca0c0a0c606dd9b44dd9ae6f3 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-patient.xlsx
+++ b/StructureDefinition-us-core-patient.xlsx
@@ -553,10 +553,10 @@
     <t>The US Core Sex Extension is used to reflect the documentation of a person's sex. It aligns with the C-CDA Sex Observation (LOINC 46098-0).</t>
   </si>
   <si>
-    <t>Patient.extension:clinical-sex</t>
-  </si>
-  <si>
-    <t>clinical-sex</t>
+    <t>Patient.extension:spfcu</t>
+  </si>
+  <si>
+    <t>spfcu</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {patient-sexParameterForClinicalUse}

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@712f58a6aaf7a6c89747fbd4fa27d755a347049f 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-patient.xlsx
+++ b/StructureDefinition-us-core-patient.xlsx
@@ -553,10 +553,10 @@
     <t>The US Core Sex Extension is used to reflect the documentation of a person's sex. It aligns with the C-CDA Sex Observation (LOINC 46098-0).</t>
   </si>
   <si>
-    <t>Patient.extension:spfcu</t>
-  </si>
-  <si>
-    <t>spfcu</t>
+    <t>Patient.extension:spcu</t>
+  </si>
+  <si>
+    <t>spcu</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {patient-sexParameterForClinicalUse}

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@0ec3e2cb932cecf594d00645bc1e641a80b718f0 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-patient.xlsx
+++ b/StructureDefinition-us-core-patient.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$96</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3607" uniqueCount="681">
   <si>
     <t>Property</t>
   </si>
@@ -626,7 +626,7 @@
 </t>
   </si>
   <si>
-    <t>Whether the patient needs an interpreter</t>
+    <t>𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜: Whether the patient needs an interpreter</t>
   </si>
   <si>
     <t>This Patient requires an interpreter to communicate healthcare information to the practitioner.</t>
@@ -1929,6 +1929,83 @@
   </si>
   <si>
     <t>PID-15, LAN-2</t>
+  </si>
+  <si>
+    <t>Patient.communication.language.id</t>
+  </si>
+  <si>
+    <t>Patient.communication.language.extension</t>
+  </si>
+  <si>
+    <t>Patient.communication.language.extension:us-core-interpreter-required</t>
+  </si>
+  <si>
+    <t>us-core-interpreter-required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/uscdi5-sandbox/StructureDefinition/us-core-interpreter-required}
+</t>
+  </si>
+  <si>
+    <t>𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜: Whether the individual needs an interpreter</t>
+  </si>
+  <si>
+    <t>This individual needs an interpreter to communicate healthcare information in the language specified in the extension's context.</t>
+  </si>
+  <si>
+    <t>The individual does not speak the default language of the organization, and hence requires an interpreter.</t>
+  </si>
+  <si>
+    <t>Patient.communication.language.coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>Patient.communication.language.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
   </si>
   <si>
     <t>Patient.communication.preferred</t>
@@ -2393,7 +2470,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO91"/>
+  <dimension ref="A1:AO96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2402,9 +2479,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.47265625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.47265625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="19.24609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="1" max="1" width="67.3515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="40.94140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="26.8359375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
@@ -2412,7 +2489,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="76.23828125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="90.953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -12086,20 +12163,16 @@
         <v>83</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>276</v>
+        <v>212</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>615</v>
+        <v>213</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>616</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>617</v>
-      </c>
-      <c r="O83" t="s" s="2">
-        <v>618</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
         <v>83</v>
       </c>
@@ -12147,7 +12220,7 @@
         <v>83</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>614</v>
+        <v>215</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>81</v>
@@ -12159,19 +12232,19 @@
         <v>83</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>619</v>
+        <v>216</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>620</v>
+        <v>83</v>
       </c>
       <c r="AM83" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>621</v>
+        <v>83</v>
       </c>
       <c r="AO83" t="s" s="2">
         <v>83</v>
@@ -12179,14 +12252,14 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>623</v>
+        <v>196</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -12205,16 +12278,16 @@
         <v>83</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>624</v>
+        <v>136</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>625</v>
+        <v>218</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>626</v>
+        <v>219</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>627</v>
+        <v>199</v>
       </c>
       <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
@@ -12252,19 +12325,19 @@
         <v>83</v>
       </c>
       <c r="AB84" t="s" s="2">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="AC84" t="s" s="2">
-        <v>83</v>
+        <v>220</v>
       </c>
       <c r="AD84" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>622</v>
+        <v>221</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>81</v>
@@ -12276,19 +12349,19 @@
         <v>83</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>628</v>
+        <v>216</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>216</v>
+        <v>83</v>
       </c>
       <c r="AM84" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AN84" t="s" s="2">
-        <v>629</v>
+        <v>83</v>
       </c>
       <c r="AO84" t="s" s="2">
         <v>83</v>
@@ -12296,12 +12369,14 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>630</v>
-      </c>
-      <c r="C85" s="2"/>
+        <v>615</v>
+      </c>
+      <c r="C85" t="s" s="2">
+        <v>617</v>
+      </c>
       <c r="D85" t="s" s="2">
         <v>83</v>
       </c>
@@ -12319,23 +12394,21 @@
         <v>83</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>268</v>
+        <v>618</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>631</v>
+        <v>619</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="N85" t="s" s="2">
-        <v>633</v>
-      </c>
-      <c r="O85" t="s" s="2">
-        <v>634</v>
-      </c>
+        <v>621</v>
+      </c>
+      <c r="O85" s="2"/>
       <c r="P85" t="s" s="2">
         <v>83</v>
       </c>
@@ -12383,25 +12456,25 @@
         <v>83</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>630</v>
+        <v>221</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>589</v>
+        <v>83</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>635</v>
+        <v>83</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>83</v>
@@ -12415,10 +12488,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12435,25 +12508,25 @@
         <v>83</v>
       </c>
       <c r="I86" t="s" s="2">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="J86" t="s" s="2">
         <v>92</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>541</v>
+        <v>623</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="N86" t="s" s="2">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="O86" t="s" s="2">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="P86" t="s" s="2">
         <v>83</v>
@@ -12502,7 +12575,7 @@
         <v>83</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>81</v>
@@ -12517,16 +12590,16 @@
         <v>103</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>641</v>
+        <v>629</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>216</v>
+        <v>83</v>
       </c>
       <c r="AM86" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>83</v>
+        <v>630</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>83</v>
@@ -12534,10 +12607,10 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12557,19 +12630,23 @@
         <v>83</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="K87" t="s" s="2">
         <v>212</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>213</v>
+        <v>632</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="N87" s="2"/>
-      <c r="O87" s="2"/>
+        <v>633</v>
+      </c>
+      <c r="N87" t="s" s="2">
+        <v>634</v>
+      </c>
+      <c r="O87" t="s" s="2">
+        <v>635</v>
+      </c>
       <c r="P87" t="s" s="2">
         <v>83</v>
       </c>
@@ -12617,7 +12694,7 @@
         <v>83</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>215</v>
+        <v>636</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>81</v>
@@ -12629,10 +12706,10 @@
         <v>83</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>216</v>
+        <v>637</v>
       </c>
       <c r="AL87" t="s" s="2">
         <v>83</v>
@@ -12641,7 +12718,7 @@
         <v>83</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>83</v>
+        <v>638</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>83</v>
@@ -12649,21 +12726,21 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
-        <v>196</v>
+        <v>83</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
         <v>81</v>
       </c>
       <c r="G88" t="s" s="2">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="H88" t="s" s="2">
         <v>83</v>
@@ -12675,18 +12752,20 @@
         <v>83</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>136</v>
+        <v>276</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>218</v>
+        <v>640</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>219</v>
+        <v>641</v>
       </c>
       <c r="N88" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="O88" s="2"/>
+        <v>642</v>
+      </c>
+      <c r="O88" t="s" s="2">
+        <v>643</v>
+      </c>
       <c r="P88" t="s" s="2">
         <v>83</v>
       </c>
@@ -12734,31 +12813,31 @@
         <v>83</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>221</v>
+        <v>639</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AH88" t="s" s="2">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="AI88" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>216</v>
+        <v>644</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>83</v>
+        <v>645</v>
       </c>
       <c r="AM88" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>83</v>
+        <v>646</v>
       </c>
       <c r="AO88" t="s" s="2">
         <v>83</v>
@@ -12766,14 +12845,14 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
-        <v>551</v>
+        <v>648</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" t="s" s="2">
@@ -12786,26 +12865,24 @@
         <v>83</v>
       </c>
       <c r="I89" t="s" s="2">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="J89" t="s" s="2">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>136</v>
+        <v>649</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>552</v>
+        <v>650</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>553</v>
+        <v>651</v>
       </c>
       <c r="N89" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="O89" t="s" s="2">
-        <v>200</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
         <v>83</v>
       </c>
@@ -12853,7 +12930,7 @@
         <v>83</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>554</v>
+        <v>647</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>81</v>
@@ -12865,19 +12942,19 @@
         <v>83</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>134</v>
+        <v>653</v>
       </c>
       <c r="AL89" t="s" s="2">
-        <v>83</v>
+        <v>216</v>
       </c>
       <c r="AM89" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>83</v>
+        <v>654</v>
       </c>
       <c r="AO89" t="s" s="2">
         <v>83</v>
@@ -12885,10 +12962,10 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12896,7 +12973,7 @@
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G90" t="s" s="2">
         <v>91</v>
@@ -12911,18 +12988,20 @@
         <v>92</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>646</v>
+        <v>268</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>649</v>
-      </c>
-      <c r="O90" s="2"/>
+        <v>658</v>
+      </c>
+      <c r="O90" t="s" s="2">
+        <v>659</v>
+      </c>
       <c r="P90" t="s" s="2">
         <v>83</v>
       </c>
@@ -12970,10 +13049,10 @@
         <v>83</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="AG90" t="s" s="2">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="AH90" t="s" s="2">
         <v>91</v>
@@ -12985,16 +13064,16 @@
         <v>103</v>
       </c>
       <c r="AK90" t="s" s="2">
-        <v>207</v>
+        <v>589</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>216</v>
+        <v>660</v>
       </c>
       <c r="AM90" t="s" s="2">
         <v>83</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>650</v>
+        <v>83</v>
       </c>
       <c r="AO90" t="s" s="2">
         <v>83</v>
@@ -13002,10 +13081,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -13013,31 +13092,35 @@
       </c>
       <c r="E91" s="2"/>
       <c r="F91" t="s" s="2">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G91" t="s" s="2">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H91" t="s" s="2">
         <v>83</v>
       </c>
       <c r="I91" t="s" s="2">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="J91" t="s" s="2">
         <v>92</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>111</v>
+        <v>541</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>653</v>
-      </c>
-      <c r="N91" s="2"/>
-      <c r="O91" s="2"/>
+        <v>663</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>664</v>
+      </c>
+      <c r="O91" t="s" s="2">
+        <v>665</v>
+      </c>
       <c r="P91" t="s" s="2">
         <v>83</v>
       </c>
@@ -13061,13 +13144,13 @@
         <v>83</v>
       </c>
       <c r="X91" t="s" s="2">
-        <v>227</v>
+        <v>83</v>
       </c>
       <c r="Y91" t="s" s="2">
-        <v>653</v>
+        <v>83</v>
       </c>
       <c r="Z91" t="s" s="2">
-        <v>654</v>
+        <v>83</v>
       </c>
       <c r="AA91" t="s" s="2">
         <v>83</v>
@@ -13085,13 +13168,13 @@
         <v>83</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AG91" t="s" s="2">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="AH91" t="s" s="2">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="AI91" t="s" s="2">
         <v>83</v>
@@ -13100,7 +13183,7 @@
         <v>103</v>
       </c>
       <c r="AK91" t="s" s="2">
-        <v>655</v>
+        <v>666</v>
       </c>
       <c r="AL91" t="s" s="2">
         <v>216</v>
@@ -13115,8 +13198,591 @@
         <v>83</v>
       </c>
     </row>
+    <row r="92" hidden="true">
+      <c r="A92" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B92" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="G92" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="M92" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Q92" s="2"/>
+      <c r="R92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AN92" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AO92" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" hidden="true">
+      <c r="A93" t="s" s="2">
+        <v>668</v>
+      </c>
+      <c r="B93" t="s" s="2">
+        <v>668</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M93" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="N93" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="O93" s="2"/>
+      <c r="P93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Q93" s="2"/>
+      <c r="R93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AN93" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AO93" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>669</v>
+      </c>
+      <c r="B94" t="s" s="2">
+        <v>669</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="O94" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="P94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Q94" s="2"/>
+      <c r="R94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AI94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ94" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AN94" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AO94" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>670</v>
+      </c>
+      <c r="B95" t="s" s="2">
+        <v>670</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>671</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>672</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>673</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>674</v>
+      </c>
+      <c r="O95" s="2"/>
+      <c r="P95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Q95" s="2"/>
+      <c r="R95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>670</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AN95" t="s" s="2">
+        <v>675</v>
+      </c>
+      <c r="AO95" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>676</v>
+      </c>
+      <c r="B96" t="s" s="2">
+        <v>676</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="E96" s="2"/>
+      <c r="F96" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>677</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+      <c r="P96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="Q96" s="2"/>
+      <c r="R96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>679</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>676</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>680</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AM96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AN96" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AO96" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AO91">
+  <autoFilter ref="A1:AO96">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -13126,7 +13792,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI90">
+  <conditionalFormatting sqref="A2:AI95">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>